<commit_message>
Bring Food Groups metadata back to MetaData file
</commit_message>
<xml_diff>
--- a/Data/Archive/MetaData.bkp.xlsx
+++ b/Data/Archive/MetaData.bkp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Majid\Documents\GitHub\IRHEIS\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Majid\Documents\GitHub\IRHEIS\Data\Archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3233F7BE-047C-4239-B2AD-10DEB540133B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C59248E-DE42-4E10-9718-E07FC1C9F949}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21691" windowHeight="15196" tabRatio="858" firstSheet="17" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="1380" windowWidth="7898" windowHeight="7380" tabRatio="858" firstSheet="55" activeTab="56" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -26549,7 +26549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -60324,7 +60324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -64190,8 +64190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>